<commit_message>
mensaje describiendo el cambio
</commit_message>
<xml_diff>
--- a/procesos/Tipo de Procesos por Responsable.xlsx
+++ b/procesos/Tipo de Procesos por Responsable.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jair/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jair/Desktop/apps procesos/procesos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F60596-C58E-B747-BB01-645DF17B435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CBFEB11-3399-0441-BA66-FDF955BDA43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2780" windowWidth="27640" windowHeight="16680" xr2:uid="{98CED4D4-BAA5-CB41-AEB8-CD9FF019EA73}"/>
+    <workbookView xWindow="4300" yWindow="2780" windowWidth="27640" windowHeight="16680" activeTab="1" xr2:uid="{98CED4D4-BAA5-CB41-AEB8-CD9FF019EA73}"/>
   </bookViews>
   <sheets>
     <sheet name="TipoProceso" sheetId="1" r:id="rId1"/>
+    <sheet name="tipo2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>AREA</t>
   </si>
@@ -162,13 +163,124 @@
   </si>
   <si>
     <t>Andres Gahona Felix</t>
+  </si>
+  <si>
+    <t>PROCESO OFICIAL (Colombia)</t>
+  </si>
+  <si>
+    <t>ESTRATÉGICO</t>
+  </si>
+  <si>
+    <t>Gestión Estratégica</t>
+  </si>
+  <si>
+    <t>Gestión Comercial y Convenios</t>
+  </si>
+  <si>
+    <t>Seguimiento y Mejora Continua</t>
+  </si>
+  <si>
+    <t>Gestión Jurídica</t>
+  </si>
+  <si>
+    <t>MISIONAL</t>
+  </si>
+  <si>
+    <t>Atención en Salud</t>
+  </si>
+  <si>
+    <t>Gestión de Farmacia</t>
+  </si>
+  <si>
+    <t>David Durán</t>
+  </si>
+  <si>
+    <t>Seguimiento en Salud</t>
+  </si>
+  <si>
+    <t>APOYO</t>
+  </si>
+  <si>
+    <t>Gestión Humana</t>
+  </si>
+  <si>
+    <t>TI / Sistemas</t>
+  </si>
+  <si>
+    <t>Gestión Administrativa</t>
+  </si>
+  <si>
+    <t>Gestión Financiera</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>MACROPROCESO (Colombia)</t>
+  </si>
+  <si>
+    <t>Acceso (Admisión/Citas)</t>
+  </si>
+  <si>
+    <t>Experiencia al Usuario</t>
+  </si>
+  <si>
+    <t>Farmacia</t>
+  </si>
+  <si>
+    <t>Almacén e Inventarios</t>
+  </si>
+  <si>
+    <t>Apoyo Diagnóstico y Terapéutico</t>
+  </si>
+  <si>
+    <t>Gestión del Talento Humano</t>
+  </si>
+  <si>
+    <t>Gestión Tecnológica e Innovación</t>
+  </si>
+  <si>
+    <t>Logística y Serv. Operativos</t>
+  </si>
+  <si>
+    <t>ÁREA LOCAL (Pestaña Perú)</t>
+  </si>
+  <si>
+    <t>RESPONSABLE / LÍDER (Perú)</t>
+  </si>
+  <si>
+    <t>Karin Alejandra Andrade</t>
+  </si>
+  <si>
+    <t>Ingrid Katherine Zapata</t>
+  </si>
+  <si>
+    <t>Wilde Lyonel Lavado</t>
+  </si>
+  <si>
+    <t>Maria Silvia Angeles</t>
+  </si>
+  <si>
+    <t>Josselyn Sharon Requena</t>
+  </si>
+  <si>
+    <t>Gianina Jessica Sigueña</t>
+  </si>
+  <si>
+    <t>Stacy Ann Carrillo</t>
+  </si>
+  <si>
+    <t>Carlos Francisco Torres</t>
+  </si>
+  <si>
+    <t>Andres Gahona</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,6 +324,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -239,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -340,11 +465,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -413,6 +553,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF527BCD-16DB-E740-B08F-0C9F3BFA426F}">
   <dimension ref="B5:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,7 +1180,7 @@
       </c>
       <c r="F27" s="21"/>
     </row>
-    <row r="28" spans="2:6" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="18" t="s">
         <v>6</v>
@@ -1048,7 +1193,7 @@
       </c>
       <c r="F28" s="21"/>
     </row>
-    <row r="29" spans="2:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="18" t="s">
         <v>13</v>
@@ -1074,7 +1219,7 @@
       </c>
       <c r="F30" s="21"/>
     </row>
-    <row r="31" spans="2:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="18" t="s">
         <v>17</v>
@@ -1087,7 +1232,7 @@
       </c>
       <c r="F31" s="21"/>
     </row>
-    <row r="32" spans="2:6" ht="91" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="18" t="s">
         <v>33</v>
@@ -1138,7 +1283,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="2:6" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="16" t="s">
         <v>0</v>
@@ -1151,7 +1296,7 @@
       </c>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="2:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="18" t="s">
         <v>19</v>
@@ -1164,7 +1309,7 @@
       </c>
       <c r="F38" s="21"/>
     </row>
-    <row r="39" spans="2:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="18" t="s">
         <v>22</v>
@@ -1177,7 +1322,7 @@
       </c>
       <c r="F39" s="21"/>
     </row>
-    <row r="40" spans="2:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="18" t="s">
         <v>24</v>
@@ -1203,7 +1348,7 @@
       </c>
       <c r="F41" s="21"/>
     </row>
-    <row r="42" spans="2:6" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="18" t="s">
         <v>29</v>
@@ -1216,7 +1361,7 @@
       </c>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="2:6" ht="61" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="18" t="s">
         <v>31</v>
@@ -1267,7 +1412,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="2:6" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="4" t="s">
         <v>0</v>
@@ -1280,7 +1425,7 @@
       </c>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="2:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="7" t="s">
         <v>8</v>
@@ -1345,4 +1490,328 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26A288F-56B8-C548-9288-8F705BCE10D6}">
+  <dimension ref="B3:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="7" width="35.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="28">
+        <v>1</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="28">
+        <v>2</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="28">
+        <v>3</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="28">
+        <v>4</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="28">
+        <v>5</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="28">
+        <v>6</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="28">
+        <v>7</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="28">
+        <v>8</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="28">
+        <v>9</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="28">
+        <v>10</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="28">
+        <v>11</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="28">
+        <v>12</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="28">
+        <v>13</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="28">
+        <v>14</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="28">
+        <v>15</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="28">
+        <v>16</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="28">
+        <v>17</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>